<commit_message>
04.05.19 Today Sales UpDated
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="19">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 30.04.19</t>
+    <t>Date: 04.05.19</t>
   </si>
 </sst>
 </file>
@@ -283,11 +283,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -298,36 +325,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,6 +332,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,6 +2253,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2265,32 +2291,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>89</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>41</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>89000</v>
+        <v>41000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>172</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>94</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>86000</v>
+        <v>47000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>300</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>30</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>30000</v>
+        <v>3000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,8 +2462,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2479,8 +2479,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2496,8 +2496,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2510,14 +2510,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>205000</v>
+        <v>91000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2560,58 +2560,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2621,11 +2621,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2712,60 +2710,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2774,10 +2772,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2792,13 +2790,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="31">
-        <v>89</v>
-      </c>
-      <c r="F33" s="31"/>
+      <c r="E33" s="34">
+        <v>41</v>
+      </c>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>89000</v>
+        <v>41000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2811,13 +2809,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="31">
-        <v>172</v>
-      </c>
-      <c r="F34" s="31"/>
+      <c r="E34" s="34">
+        <v>94</v>
+      </c>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>86000</v>
+        <v>47000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2830,13 +2828,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="31">
-        <v>300</v>
-      </c>
-      <c r="F35" s="31"/>
+      <c r="E35" s="34">
+        <v>30</v>
+      </c>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>3000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2849,8 +2847,8 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2866,8 +2864,8 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -2883,8 +2881,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2897,14 +2895,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>205000</v>
+        <v>91000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2947,58 +2945,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3008,11 +3006,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3040,6 +3036,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3056,28 +3074,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3108,63 +3104,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3174,10 +3170,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3192,10 +3188,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3211,10 +3207,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3230,10 +3226,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3249,10 +3245,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3268,10 +3264,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3287,8 +3283,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3301,10 +3297,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3351,60 +3347,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3416,11 +3412,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3495,60 +3491,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3557,10 +3553,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3575,10 +3571,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3594,10 +3590,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3613,10 +3609,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3632,10 +3628,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3651,10 +3647,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3670,8 +3666,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3734,60 +3730,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3799,11 +3795,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3831,6 +3827,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3847,30 +3867,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3902,63 +3898,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3968,10 +3964,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3986,10 +3982,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4005,10 +4001,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4024,10 +4020,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4043,8 +4039,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4060,8 +4056,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4077,8 +4073,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4091,10 +4087,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4141,72 +4137,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4281,60 +4277,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4343,10 +4339,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4361,10 +4357,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4380,10 +4376,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4399,10 +4395,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4418,8 +4414,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4435,8 +4431,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4452,8 +4448,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4466,10 +4462,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4516,58 +4512,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4577,11 +4573,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4609,16 +4605,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4631,24 +4635,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
07.05.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 04.05.19</t>
+    <t>Date: 07.05.19</t>
   </si>
 </sst>
 </file>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection sqref="A1:J47"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2406,12 +2406,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="21">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>41000</v>
+        <v>45000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2425,12 +2425,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="21">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>47000</v>
+        <v>29500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2444,12 +2444,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="21">
-        <v>30</v>
+        <v>146</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>14600</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,11 +2462,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="21">
+        <v>100</v>
+      </c>
       <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2479,11 +2481,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="21">
+        <v>45</v>
+      </c>
       <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2517,7 +2521,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>91000</v>
+        <v>95000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2791,12 +2795,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="34">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>41000</v>
+        <v>45000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2810,12 +2814,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="34">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>47000</v>
+        <v>29500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2829,12 +2833,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="34">
-        <v>30</v>
+        <v>146</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>14600</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2847,11 +2851,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
+      <c r="E36" s="34">
+        <v>100</v>
+      </c>
       <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2864,11 +2870,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34"/>
+      <c r="E37" s="34">
+        <v>45</v>
+      </c>
       <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2902,7 +2910,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>91000</v>
+        <v>95000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>

</xml_diff>

<commit_message>
11.05.19 Today Sales Updated 12:13PM
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 08.05.19</t>
+    <t>Date: 09.05.19</t>
   </si>
 </sst>
 </file>
@@ -283,11 +283,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -298,36 +325,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,6 +332,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,6 +2253,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2265,32 +2291,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection sqref="A1:J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>46</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>15</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>46000</v>
+        <v>15000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>130</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>73</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>65000</v>
+        <v>36500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>84</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>389</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>8400</v>
+        <v>38900</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,13 +2462,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
-        <v>5</v>
-      </c>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21">
+        <v>76</v>
+      </c>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>3800</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2481,11 +2481,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21">
+        <v>190</v>
+      </c>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3800</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2498,13 +2500,13 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23">
-        <v>35</v>
-      </c>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21">
+        <v>100</v>
+      </c>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>350</v>
+        <v>1000</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2514,14 +2516,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>120000</v>
+        <v>99000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2564,58 +2566,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2625,9 +2627,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2714,60 +2716,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2776,10 +2778,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2794,13 +2796,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="31">
-        <v>46</v>
-      </c>
-      <c r="F33" s="31"/>
+      <c r="E33" s="34">
+        <v>15</v>
+      </c>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>46000</v>
+        <v>15000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2813,13 +2815,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="31">
-        <v>130</v>
-      </c>
-      <c r="F34" s="31"/>
+      <c r="E34" s="34">
+        <v>73</v>
+      </c>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>65000</v>
+        <v>36500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2832,13 +2834,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="31">
-        <v>84</v>
-      </c>
-      <c r="F35" s="31"/>
+      <c r="E35" s="34">
+        <v>389</v>
+      </c>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>8400</v>
+        <v>38900</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2851,13 +2853,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="31">
-        <v>5</v>
-      </c>
-      <c r="F36" s="31"/>
+      <c r="E36" s="34">
+        <v>76</v>
+      </c>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>250</v>
+        <v>3800</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2870,11 +2872,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34">
+        <v>190</v>
+      </c>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>3800</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2887,13 +2891,13 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31">
-        <v>35</v>
-      </c>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34">
+        <v>100</v>
+      </c>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>350</v>
+        <v>1000</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2903,14 +2907,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>120000</v>
+        <v>99000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2953,58 +2957,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3014,9 +3018,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3044,6 +3048,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3060,28 +3086,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3112,63 +3116,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3178,10 +3182,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3196,10 +3200,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3215,10 +3219,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3234,10 +3238,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3253,10 +3257,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3272,10 +3276,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3291,8 +3295,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3305,10 +3309,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3355,60 +3359,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3420,11 +3424,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3499,60 +3503,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3561,10 +3565,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3579,10 +3583,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3598,10 +3602,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3617,10 +3621,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3636,10 +3640,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3655,10 +3659,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3674,8 +3678,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3738,60 +3742,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3803,11 +3807,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3835,6 +3839,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3851,30 +3879,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3906,63 +3910,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3972,10 +3976,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3990,10 +3994,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4009,10 +4013,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4028,10 +4032,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4047,8 +4051,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4064,8 +4068,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4081,8 +4085,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4095,10 +4099,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4145,72 +4149,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4285,60 +4289,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4347,10 +4351,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4365,10 +4369,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4384,10 +4388,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4403,10 +4407,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4422,8 +4426,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4439,8 +4443,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4456,8 +4460,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4470,10 +4474,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4520,58 +4524,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4581,11 +4585,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4613,16 +4617,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4635,24 +4647,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
11.05.19 Today Sales Updated 11:14PM
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 09.05.19</t>
+    <t>Date: 11.05.19</t>
   </si>
 </sst>
 </file>
@@ -283,38 +283,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -325,6 +298,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -332,9 +335,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,14 +2253,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2273,24 +2283,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2303,7 +2303,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection sqref="A1:J48"/>
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>15</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>70</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>15000</v>
+        <v>70000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>73</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>109</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>36500</v>
+        <v>54500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>389</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>215</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>38900</v>
+        <v>21500</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,13 +2462,11 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
-        <v>76</v>
-      </c>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>3800</v>
+        <v>0</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2481,13 +2479,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
-        <v>190</v>
-      </c>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>3800</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2500,13 +2496,11 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21">
-        <v>100</v>
-      </c>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2516,14 +2510,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>99000</v>
+        <v>146000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2566,58 +2560,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2627,9 +2621,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2716,60 +2710,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2778,10 +2772,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2796,13 +2790,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
-        <v>15</v>
-      </c>
-      <c r="F33" s="34"/>
+      <c r="E33" s="31">
+        <v>70</v>
+      </c>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>15000</v>
+        <v>70000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2815,13 +2809,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
-        <v>73</v>
-      </c>
-      <c r="F34" s="34"/>
+      <c r="E34" s="31">
+        <v>109</v>
+      </c>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>36500</v>
+        <v>54500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2834,13 +2828,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
-        <v>389</v>
-      </c>
-      <c r="F35" s="34"/>
+      <c r="E35" s="31">
+        <v>215</v>
+      </c>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>38900</v>
+        <v>21500</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2853,13 +2847,11 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="34">
-        <v>76</v>
-      </c>
-      <c r="F36" s="34"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>3800</v>
+        <v>0</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2872,13 +2864,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34">
-        <v>190</v>
-      </c>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>3800</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2891,13 +2881,11 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34">
-        <v>100</v>
-      </c>
-      <c r="F38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2907,14 +2895,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>99000</v>
+        <v>146000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2957,58 +2945,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3018,9 +3006,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3048,28 +3036,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3086,6 +3052,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3116,63 +3104,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3182,10 +3170,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3200,10 +3188,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3219,10 +3207,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3238,10 +3226,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3257,10 +3245,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3276,10 +3264,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3295,8 +3283,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3309,10 +3297,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3359,60 +3347,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3424,11 +3412,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3503,60 +3491,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3565,10 +3553,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3583,10 +3571,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3602,10 +3590,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3621,10 +3609,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3640,10 +3628,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3659,10 +3647,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3678,8 +3666,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3742,60 +3730,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3807,11 +3795,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3839,30 +3827,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3879,6 +3843,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3910,63 +3898,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3976,10 +3964,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3994,10 +3982,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4013,10 +4001,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4032,10 +4020,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4051,8 +4039,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4068,8 +4056,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4085,8 +4073,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4099,10 +4087,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4149,72 +4137,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4289,60 +4277,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4351,10 +4339,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4369,10 +4357,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4388,10 +4376,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4407,10 +4395,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4426,8 +4414,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4443,8 +4431,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4460,8 +4448,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4474,10 +4462,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4524,58 +4512,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4585,11 +4573,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4617,6 +4605,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4629,34 +4645,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
12.05.19 Today Sales Updated 10:22PM
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 11.05.19</t>
+    <t>Date: 12.05.19</t>
   </si>
 </sst>
 </file>
@@ -283,11 +283,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -298,36 +325,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,6 +332,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,6 +2253,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2265,32 +2291,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>70</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>26</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>70000</v>
+        <v>26000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>109</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>200</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>54500</v>
+        <v>100000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>215</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>300</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>21500</v>
+        <v>30000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,8 +2462,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2479,8 +2479,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2496,8 +2496,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2510,14 +2510,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>146000</v>
+        <v>156000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2560,58 +2560,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2621,9 +2621,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2710,60 +2710,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2772,10 +2772,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2790,13 +2790,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="31">
-        <v>70</v>
-      </c>
-      <c r="F33" s="31"/>
+      <c r="E33" s="34">
+        <v>26</v>
+      </c>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>70000</v>
+        <v>26000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2809,13 +2809,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="31">
-        <v>109</v>
-      </c>
-      <c r="F34" s="31"/>
+      <c r="E34" s="34">
+        <v>200</v>
+      </c>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>54500</v>
+        <v>100000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2828,13 +2828,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="31">
-        <v>215</v>
-      </c>
-      <c r="F35" s="31"/>
+      <c r="E35" s="34">
+        <v>300</v>
+      </c>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>21500</v>
+        <v>30000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2847,8 +2847,8 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2864,8 +2864,8 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -2881,8 +2881,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2895,14 +2895,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>146000</v>
+        <v>156000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2945,58 +2945,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3006,9 +3006,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3036,6 +3036,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3052,28 +3074,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3104,63 +3104,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3170,10 +3170,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3188,10 +3188,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3207,10 +3207,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3226,10 +3226,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3245,10 +3245,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3264,10 +3264,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3283,8 +3283,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3297,10 +3297,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3347,60 +3347,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3412,11 +3412,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3491,60 +3491,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3553,10 +3553,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3571,10 +3571,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3590,10 +3590,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3609,10 +3609,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3628,10 +3628,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3647,10 +3647,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3666,8 +3666,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3730,60 +3730,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3795,11 +3795,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3827,6 +3827,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3843,30 +3867,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3898,63 +3898,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3964,10 +3964,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3982,10 +3982,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4001,10 +4001,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4020,10 +4020,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4039,8 +4039,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4056,8 +4056,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4073,8 +4073,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4087,10 +4087,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4137,72 +4137,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4277,60 +4277,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4339,10 +4339,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4357,10 +4357,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4376,10 +4376,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4395,10 +4395,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4414,8 +4414,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4431,8 +4431,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4448,8 +4448,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4462,10 +4462,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4512,58 +4512,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4573,11 +4573,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4605,16 +4605,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4627,24 +4635,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
19.05.19 Today Sales Updated
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 18.05.19</t>
+    <t>Date: 19.05.19</t>
   </si>
 </sst>
 </file>
@@ -283,38 +283,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -325,6 +298,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -332,9 +335,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,14 +2253,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2273,24 +2283,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection sqref="A1:J47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H47" sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>70</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>37</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>70000</v>
+        <v>37000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>106</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>110</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>53000</v>
+        <v>55000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>210</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>91</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>21000</v>
+        <v>9100</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,13 +2462,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
-        <v>100</v>
-      </c>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23">
+        <v>46</v>
+      </c>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>2300</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2481,11 +2481,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23">
+        <v>30</v>
+      </c>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2498,8 +2500,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2512,14 +2514,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>149000</v>
+        <v>104000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2562,58 +2564,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2623,9 +2625,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2712,60 +2714,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2774,10 +2776,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2792,13 +2794,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
-        <v>70</v>
-      </c>
-      <c r="F33" s="34"/>
+      <c r="E33" s="31">
+        <v>37</v>
+      </c>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>70000</v>
+        <v>37000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2811,13 +2813,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
-        <v>106</v>
-      </c>
-      <c r="F34" s="34"/>
+      <c r="E34" s="31">
+        <v>110</v>
+      </c>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>53000</v>
+        <v>55000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2830,13 +2832,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
-        <v>210</v>
-      </c>
-      <c r="F35" s="34"/>
+      <c r="E35" s="31">
+        <v>91</v>
+      </c>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>21000</v>
+        <v>9100</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2849,13 +2851,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="34">
-        <v>100</v>
-      </c>
-      <c r="F36" s="34"/>
+      <c r="E36" s="31">
+        <v>46</v>
+      </c>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>2300</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2868,11 +2870,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31">
+        <v>30</v>
+      </c>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2885,8 +2889,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2899,14 +2903,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>149000</v>
+        <v>104000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2949,58 +2953,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3010,9 +3014,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3040,28 +3044,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3078,6 +3060,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3108,63 +3112,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3174,10 +3178,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3192,10 +3196,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3211,10 +3215,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3230,10 +3234,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3249,10 +3253,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3268,10 +3272,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3287,8 +3291,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3301,10 +3305,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3351,60 +3355,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3416,11 +3420,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3495,60 +3499,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3557,10 +3561,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3575,10 +3579,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3594,10 +3598,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3613,10 +3617,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3632,10 +3636,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3651,10 +3655,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3670,8 +3674,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3734,60 +3738,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3799,11 +3803,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3831,30 +3835,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3871,6 +3851,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3902,63 +3906,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3968,10 +3972,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3986,10 +3990,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4005,10 +4009,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4024,10 +4028,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4043,8 +4047,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4060,8 +4064,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4077,8 +4081,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4091,10 +4095,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4141,72 +4145,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4281,60 +4285,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4343,10 +4347,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4361,10 +4365,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4380,10 +4384,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4399,10 +4403,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4418,8 +4422,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4435,8 +4439,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4452,8 +4456,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4466,10 +4470,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4516,58 +4520,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4577,11 +4581,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4609,6 +4613,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4621,34 +4653,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
20.05.19 Today Sales Details 10:51PM
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 19.05.19</t>
+    <t>Date: 20.05.19</t>
   </si>
 </sst>
 </file>
@@ -283,11 +283,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -298,36 +325,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,6 +332,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,6 +2253,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2265,32 +2291,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="A1:J47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>37</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>20</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>37000</v>
+        <v>20000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>110</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>109</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>55000</v>
+        <v>54500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>91</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>175</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>9100</v>
+        <v>17500</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,13 +2462,11 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
-        <v>46</v>
-      </c>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2481,13 +2479,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
-        <v>30</v>
-      </c>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2500,11 +2496,13 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21">
+        <v>100</v>
+      </c>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2514,14 +2512,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>104000</v>
+        <v>93000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2564,58 +2562,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2625,9 +2623,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2714,60 +2712,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2776,10 +2774,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2794,13 +2792,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="31">
-        <v>37</v>
-      </c>
-      <c r="F33" s="31"/>
+      <c r="E33" s="34">
+        <v>20</v>
+      </c>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>37000</v>
+        <v>20000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2813,13 +2811,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="31">
-        <v>110</v>
-      </c>
-      <c r="F34" s="31"/>
+      <c r="E34" s="34">
+        <v>109</v>
+      </c>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>55000</v>
+        <v>54500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2832,13 +2830,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="31">
-        <v>91</v>
-      </c>
-      <c r="F35" s="31"/>
+      <c r="E35" s="34">
+        <v>175</v>
+      </c>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>9100</v>
+        <v>17500</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2851,13 +2849,11 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="31">
-        <v>46</v>
-      </c>
-      <c r="F36" s="31"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2870,13 +2866,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31">
-        <v>30</v>
-      </c>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2889,11 +2883,13 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34">
+        <v>100</v>
+      </c>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2903,14 +2899,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>104000</v>
+        <v>93000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2953,58 +2949,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3014,9 +3010,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3044,6 +3040,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3060,28 +3078,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3112,63 +3108,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3178,10 +3174,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3196,10 +3192,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3215,10 +3211,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3234,10 +3230,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3253,10 +3249,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3272,10 +3268,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3291,8 +3287,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3305,10 +3301,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3355,60 +3351,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3420,11 +3416,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3499,60 +3495,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3561,10 +3557,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3579,10 +3575,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3598,10 +3594,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3617,10 +3613,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3636,10 +3632,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3655,10 +3651,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3674,8 +3670,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3738,60 +3734,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3803,11 +3799,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3835,6 +3831,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3851,30 +3871,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3906,63 +3902,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3972,10 +3968,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3990,10 +3986,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4009,10 +4005,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4028,10 +4024,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4047,8 +4043,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4064,8 +4060,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4081,8 +4077,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4095,10 +4091,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4145,72 +4141,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4285,60 +4281,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4347,10 +4343,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4365,10 +4361,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4384,10 +4380,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4403,10 +4399,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4422,8 +4418,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4439,8 +4435,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4456,8 +4452,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4470,10 +4466,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4520,58 +4516,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4581,11 +4577,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4613,16 +4609,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4635,24 +4639,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
21.05.19 Today Last Sales Updated
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 20.05.19</t>
+    <t>Date: 21.05.19</t>
   </si>
 </sst>
 </file>
@@ -283,38 +283,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -325,6 +298,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -332,9 +335,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,14 +2253,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2273,24 +2283,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>20</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>70</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>20000</v>
+        <v>70000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>109</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>76</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>54500</v>
+        <v>38000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>175</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>100</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>17500</v>
+        <v>10000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,11 +2462,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23">
+        <v>20</v>
+      </c>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2479,8 +2481,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2496,13 +2498,11 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21">
-        <v>100</v>
-      </c>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2512,14 +2512,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>93000</v>
+        <v>119000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2562,58 +2562,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2623,9 +2623,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2712,60 +2712,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2774,10 +2774,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2792,13 +2792,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
-        <v>20</v>
-      </c>
-      <c r="F33" s="34"/>
+      <c r="E33" s="31">
+        <v>70</v>
+      </c>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>20000</v>
+        <v>70000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2811,13 +2811,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
-        <v>109</v>
-      </c>
-      <c r="F34" s="34"/>
+      <c r="E34" s="31">
+        <v>76</v>
+      </c>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>54500</v>
+        <v>38000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2830,13 +2830,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
-        <v>175</v>
-      </c>
-      <c r="F35" s="34"/>
+      <c r="E35" s="31">
+        <v>100</v>
+      </c>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>17500</v>
+        <v>10000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2849,11 +2849,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="31">
+        <v>20</v>
+      </c>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2866,8 +2868,8 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -2883,13 +2885,11 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34">
-        <v>100</v>
-      </c>
-      <c r="F38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2899,14 +2899,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>93000</v>
+        <v>119000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2949,58 +2949,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3010,9 +3010,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3040,28 +3040,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3078,6 +3056,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3108,63 +3108,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3174,10 +3174,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3192,10 +3192,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3211,10 +3211,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3230,10 +3230,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3249,10 +3249,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3268,10 +3268,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3287,8 +3287,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3301,10 +3301,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3351,60 +3351,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3416,11 +3416,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3495,60 +3495,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3557,10 +3557,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3575,10 +3575,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3594,10 +3594,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3613,10 +3613,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3632,10 +3632,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3651,10 +3651,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3670,8 +3670,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3734,60 +3734,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3799,11 +3799,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3831,30 +3831,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3871,6 +3847,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3902,63 +3902,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3968,10 +3968,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3986,10 +3986,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4005,10 +4005,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4024,10 +4024,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4043,8 +4043,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4060,8 +4060,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4077,8 +4077,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4091,10 +4091,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4141,72 +4141,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4281,60 +4281,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4343,10 +4343,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4361,10 +4361,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4380,10 +4380,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4399,10 +4399,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4418,8 +4418,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4435,8 +4435,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4452,8 +4452,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4466,10 +4466,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4516,58 +4516,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4577,11 +4577,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4609,6 +4609,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4621,34 +4649,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
23.05.19 Today Sales Updated 11:06 PM
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 21.05.19</t>
+    <t>Date: 22.05.19</t>
   </si>
 </sst>
 </file>
@@ -283,11 +283,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -298,36 +325,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,6 +332,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,6 +2253,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2265,32 +2291,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection sqref="A1:J47"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>70</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>48</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>70000</v>
+        <v>48000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>76</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>151</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>38000</v>
+        <v>75500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>100</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>105</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>10500</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,13 +2462,11 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
-        <v>20</v>
-      </c>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2481,8 +2479,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2498,8 +2496,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2512,14 +2510,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>119000</v>
+        <v>134000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2562,58 +2560,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2623,9 +2621,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2712,60 +2710,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2774,10 +2772,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2792,13 +2790,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="31">
-        <v>70</v>
-      </c>
-      <c r="F33" s="31"/>
+      <c r="E33" s="34">
+        <v>48</v>
+      </c>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>70000</v>
+        <v>48000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2811,13 +2809,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="31">
-        <v>76</v>
-      </c>
-      <c r="F34" s="31"/>
+      <c r="E34" s="34">
+        <v>151</v>
+      </c>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>38000</v>
+        <v>75500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2830,13 +2828,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="31">
-        <v>100</v>
-      </c>
-      <c r="F35" s="31"/>
+      <c r="E35" s="34">
+        <v>105</v>
+      </c>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>10500</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2849,13 +2847,11 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="31">
-        <v>20</v>
-      </c>
-      <c r="F36" s="31"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2868,8 +2864,8 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -2885,8 +2881,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2899,14 +2895,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>119000</v>
+        <v>134000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2949,58 +2945,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3010,9 +3006,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3040,6 +3036,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3056,28 +3074,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3108,63 +3104,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3174,10 +3170,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3192,10 +3188,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3211,10 +3207,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3230,10 +3226,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3249,10 +3245,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3268,10 +3264,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3287,8 +3283,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3301,10 +3297,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3351,60 +3347,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3416,11 +3412,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3495,60 +3491,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3557,10 +3553,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3575,10 +3571,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3594,10 +3590,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3613,10 +3609,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3632,10 +3628,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3651,10 +3647,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3670,8 +3666,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3734,60 +3730,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3799,11 +3795,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3831,6 +3827,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3847,30 +3867,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3902,63 +3898,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3968,10 +3964,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3986,10 +3982,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4005,10 +4001,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4024,10 +4020,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4043,8 +4039,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4060,8 +4056,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4077,8 +4073,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4091,10 +4087,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4141,72 +4137,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4281,60 +4277,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4343,10 +4339,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4361,10 +4357,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4380,10 +4376,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4399,10 +4395,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4418,8 +4414,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4435,8 +4431,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4452,8 +4448,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4466,10 +4462,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4516,58 +4512,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4577,11 +4573,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4609,16 +4605,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4631,24 +4635,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
25.05.19 Today Last Sales Updated 11:10PM
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 22.05.19</t>
+    <t>Date: 25.05.19</t>
   </si>
 </sst>
 </file>
@@ -283,38 +283,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -325,6 +298,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -332,9 +335,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,14 +2253,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2273,24 +2283,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K47" sqref="A1:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>48</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>100</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>48000</v>
+        <v>100000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>151</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>72</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>75500</v>
+        <v>36000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>105</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>910</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>10500</v>
+        <v>91000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,8 +2462,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2479,8 +2479,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2496,8 +2496,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2510,14 +2510,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>134000</v>
+        <v>227000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2560,58 +2560,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2621,9 +2621,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2710,60 +2710,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2772,10 +2772,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2790,13 +2790,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
-        <v>48</v>
-      </c>
-      <c r="F33" s="34"/>
+      <c r="E33" s="31">
+        <v>100</v>
+      </c>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>48000</v>
+        <v>100000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2809,13 +2809,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
-        <v>151</v>
-      </c>
-      <c r="F34" s="34"/>
+      <c r="E34" s="31">
+        <v>72</v>
+      </c>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>75500</v>
+        <v>36000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2828,13 +2828,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
-        <v>105</v>
-      </c>
-      <c r="F35" s="34"/>
+      <c r="E35" s="31">
+        <v>910</v>
+      </c>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>10500</v>
+        <v>91000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2847,8 +2847,8 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2864,8 +2864,8 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -2881,8 +2881,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2895,14 +2895,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>134000</v>
+        <v>227000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2945,58 +2945,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3006,9 +3006,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3036,28 +3036,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3074,6 +3052,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3104,63 +3104,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3170,10 +3170,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3188,10 +3188,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3207,10 +3207,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3226,10 +3226,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3245,10 +3245,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3264,10 +3264,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3283,8 +3283,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3297,10 +3297,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3347,60 +3347,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3412,11 +3412,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3491,60 +3491,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3553,10 +3553,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3571,10 +3571,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3590,10 +3590,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3609,10 +3609,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3628,10 +3628,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3647,10 +3647,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3666,8 +3666,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3730,60 +3730,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3795,11 +3795,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3827,30 +3827,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3867,6 +3843,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3898,63 +3898,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3964,10 +3964,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3982,10 +3982,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4001,10 +4001,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4020,10 +4020,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4039,8 +4039,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4056,8 +4056,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4073,8 +4073,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4087,10 +4087,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4137,72 +4137,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4277,60 +4277,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4339,10 +4339,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4357,10 +4357,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4376,10 +4376,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4395,10 +4395,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4414,8 +4414,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4431,8 +4431,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4448,8 +4448,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4462,10 +4462,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4512,58 +4512,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4573,11 +4573,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4605,6 +4605,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4617,34 +4645,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
26.05.19 Today Last 11:53PM Sales updated
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 25.05.19</t>
+    <t>Date: 26.05.19</t>
   </si>
 </sst>
 </file>
@@ -283,11 +283,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -298,36 +325,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,6 +332,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,6 +2253,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2265,32 +2291,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>100</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>25</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>100000</v>
+        <v>25000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>72</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>206</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>36000</v>
+        <v>103000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>910</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>417</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>91000</v>
+        <v>41700</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,11 +2462,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21">
+        <v>126</v>
+      </c>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6300</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2479,8 +2481,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2496,8 +2498,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2510,14 +2512,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>227000</v>
+        <v>176000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2560,58 +2562,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2621,9 +2623,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2710,60 +2712,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2772,10 +2774,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2790,13 +2792,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="31">
-        <v>100</v>
-      </c>
-      <c r="F33" s="31"/>
+      <c r="E33" s="21">
+        <v>25</v>
+      </c>
+      <c r="F33" s="21"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>100000</v>
+        <v>25000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2809,13 +2811,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="31">
-        <v>72</v>
-      </c>
-      <c r="F34" s="31"/>
+      <c r="E34" s="21">
+        <v>206</v>
+      </c>
+      <c r="F34" s="21"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>36000</v>
+        <v>103000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2828,13 +2830,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="31">
-        <v>910</v>
-      </c>
-      <c r="F35" s="31"/>
+      <c r="E35" s="21">
+        <v>417</v>
+      </c>
+      <c r="F35" s="21"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>91000</v>
+        <v>41700</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2847,11 +2849,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
+      <c r="E36" s="21">
+        <v>126</v>
+      </c>
+      <c r="F36" s="21"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6300</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2864,8 +2868,8 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -2881,8 +2885,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2895,14 +2899,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>227000</v>
+        <v>176000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2945,58 +2949,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3006,9 +3010,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3036,6 +3040,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3052,28 +3078,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3104,63 +3108,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3170,10 +3174,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3188,10 +3192,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3207,10 +3211,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3226,10 +3230,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3245,10 +3249,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3264,10 +3268,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3283,8 +3287,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3297,10 +3301,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3347,60 +3351,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3412,11 +3416,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3491,60 +3495,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3553,10 +3557,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3571,10 +3575,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3590,10 +3594,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3609,10 +3613,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3628,10 +3632,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3647,10 +3651,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3666,8 +3670,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3730,60 +3734,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3795,11 +3799,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3827,6 +3831,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3843,30 +3871,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3898,63 +3902,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3964,10 +3968,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3982,10 +3986,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4001,10 +4005,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4020,10 +4024,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4039,8 +4043,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4056,8 +4060,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4073,8 +4077,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4087,10 +4091,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4137,72 +4141,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4277,60 +4281,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4339,10 +4343,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4357,10 +4361,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4376,10 +4380,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4395,10 +4399,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4414,8 +4418,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4431,8 +4435,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4448,8 +4452,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4462,10 +4466,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4512,58 +4516,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4573,11 +4577,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4605,16 +4609,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4627,24 +4639,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
29.05.19 Today Last Sales Updated 11:11 PM
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 28.05.19</t>
+    <t>Date: 29.05.19</t>
   </si>
 </sst>
 </file>
@@ -283,11 +283,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -298,36 +325,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,6 +332,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,6 +2253,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2265,32 +2291,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="A1:J47"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>44</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>56</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>44000</v>
+        <v>56000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>278</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>279</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>139000</v>
+        <v>139500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>320</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>295</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>32000</v>
+        <v>29500</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,8 +2462,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2479,8 +2479,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2496,8 +2496,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2510,14 +2510,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>215000</v>
+        <v>225000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2560,58 +2560,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2621,9 +2621,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2710,60 +2710,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2772,10 +2772,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2790,13 +2790,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="23">
-        <v>44</v>
-      </c>
-      <c r="F33" s="23"/>
+      <c r="E33" s="21">
+        <v>56</v>
+      </c>
+      <c r="F33" s="21"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>44000</v>
+        <v>56000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2809,13 +2809,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="23">
-        <v>278</v>
-      </c>
-      <c r="F34" s="23"/>
+      <c r="E34" s="21">
+        <v>279</v>
+      </c>
+      <c r="F34" s="21"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>139000</v>
+        <v>139500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2828,13 +2828,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="23">
-        <v>320</v>
-      </c>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21">
+        <v>295</v>
+      </c>
+      <c r="F35" s="21"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>32000</v>
+        <v>29500</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2847,8 +2847,8 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2864,8 +2864,8 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -2881,8 +2881,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2895,14 +2895,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>215000</v>
+        <v>225000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2945,58 +2945,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3006,9 +3006,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3036,6 +3036,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3052,28 +3074,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3104,63 +3104,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3170,10 +3170,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3188,10 +3188,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3207,10 +3207,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3226,10 +3226,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3245,10 +3245,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3264,10 +3264,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3283,8 +3283,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3297,10 +3297,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3347,60 +3347,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3412,11 +3412,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3491,60 +3491,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3553,10 +3553,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3571,10 +3571,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3590,10 +3590,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3609,10 +3609,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3628,10 +3628,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3647,10 +3647,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3666,8 +3666,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3730,60 +3730,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3795,11 +3795,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3827,6 +3827,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3843,30 +3867,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3898,63 +3898,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3964,10 +3964,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3982,10 +3982,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4001,10 +4001,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4020,10 +4020,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4039,8 +4039,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4056,8 +4056,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4073,8 +4073,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4087,10 +4087,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4137,72 +4137,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4277,60 +4277,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4339,10 +4339,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4357,10 +4357,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4376,10 +4376,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4395,10 +4395,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4414,8 +4414,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4431,8 +4431,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4448,8 +4448,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4462,10 +4462,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4512,58 +4512,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4573,11 +4573,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4605,16 +4605,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4627,24 +4635,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
08.06.19 Today Sales Updated 1:44am
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 04.06.19</t>
+    <t>Date: 08.06.19</t>
   </si>
 </sst>
 </file>
@@ -283,38 +283,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -325,6 +298,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -332,9 +335,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,14 +2253,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2273,24 +2283,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection sqref="A1:J47"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>85</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>186</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>85000</v>
+        <v>186000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>204</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>700</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>102000</v>
+        <v>350000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>170</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>500</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>17000</v>
+        <v>50000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,11 +2462,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23">
+        <v>20</v>
+      </c>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2479,8 +2481,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2496,8 +2498,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2510,14 +2512,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>204000</v>
+        <v>587000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2560,58 +2562,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2621,9 +2623,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2710,60 +2712,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2772,10 +2774,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2790,13 +2792,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="21">
-        <v>85</v>
-      </c>
-      <c r="F33" s="21"/>
+      <c r="E33" s="23">
+        <v>186</v>
+      </c>
+      <c r="F33" s="23"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>85000</v>
+        <v>186000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2809,13 +2811,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="21">
-        <v>204</v>
-      </c>
-      <c r="F34" s="21"/>
+      <c r="E34" s="23">
+        <v>700</v>
+      </c>
+      <c r="F34" s="23"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>102000</v>
+        <v>350000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2828,13 +2830,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="21">
-        <v>170</v>
-      </c>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23">
+        <v>500</v>
+      </c>
+      <c r="F35" s="23"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>17000</v>
+        <v>50000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2847,11 +2849,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23">
+        <v>20</v>
+      </c>
+      <c r="F36" s="23"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2864,8 +2868,8 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -2881,8 +2885,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2895,14 +2899,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>204000</v>
+        <v>587000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2945,58 +2949,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3006,9 +3010,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3036,28 +3040,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3074,6 +3056,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3104,63 +3108,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3170,10 +3174,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3188,10 +3192,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3207,10 +3211,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3226,10 +3230,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3245,10 +3249,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3264,10 +3268,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3283,8 +3287,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3297,10 +3301,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3347,60 +3351,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3412,11 +3416,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3491,60 +3495,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3553,10 +3557,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3571,10 +3575,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3590,10 +3594,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3609,10 +3613,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3628,10 +3632,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3647,10 +3651,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3666,8 +3670,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3730,60 +3734,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3795,11 +3799,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3827,30 +3831,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3867,6 +3847,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3898,63 +3902,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3964,10 +3968,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3982,10 +3986,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4001,10 +4005,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4020,10 +4024,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4039,8 +4043,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4056,8 +4060,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4073,8 +4077,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4087,10 +4091,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4137,72 +4141,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4277,60 +4281,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4339,10 +4343,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4357,10 +4361,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4376,10 +4380,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4395,10 +4399,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4414,8 +4418,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4431,8 +4435,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4448,8 +4452,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4462,10 +4466,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4512,58 +4516,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4573,11 +4577,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4605,6 +4609,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4617,34 +4649,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
11.06.19 Sales Updated 11:23 PM
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 10.06.19</t>
+    <t>Date: 11.06.19</t>
   </si>
 </sst>
 </file>
@@ -283,11 +283,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -298,36 +325,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,6 +332,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,6 +2253,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2265,32 +2291,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="A1:J47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>86</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>43</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>86000</v>
+        <v>43000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>312</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>212</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>156000</v>
+        <v>106000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>530</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>214</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>53000</v>
+        <v>21400</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,13 +2462,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
-        <v>140</v>
-      </c>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21">
+        <v>132</v>
+      </c>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>7000</v>
+        <v>6600</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2481,8 +2481,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2498,8 +2498,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2512,14 +2512,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>302000</v>
+        <v>177000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2562,58 +2562,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2623,9 +2623,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2712,60 +2712,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2774,10 +2774,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2792,13 +2792,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="23">
-        <v>86</v>
-      </c>
-      <c r="F33" s="23"/>
+      <c r="E33" s="21">
+        <v>43</v>
+      </c>
+      <c r="F33" s="21"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>86000</v>
+        <v>43000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2811,13 +2811,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="23">
-        <v>312</v>
-      </c>
-      <c r="F34" s="23"/>
+      <c r="E34" s="21">
+        <v>212</v>
+      </c>
+      <c r="F34" s="21"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>156000</v>
+        <v>106000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2830,13 +2830,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="23">
-        <v>530</v>
-      </c>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21">
+        <v>214</v>
+      </c>
+      <c r="F35" s="21"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>53000</v>
+        <v>21400</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2849,13 +2849,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="23">
-        <v>140</v>
-      </c>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21">
+        <v>132</v>
+      </c>
+      <c r="F36" s="21"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>7000</v>
+        <v>6600</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2868,8 +2868,8 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -2885,8 +2885,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2899,14 +2899,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>302000</v>
+        <v>177000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2949,58 +2949,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3010,9 +3010,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3040,6 +3040,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3056,28 +3078,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3108,63 +3108,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3174,10 +3174,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3192,10 +3192,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3211,10 +3211,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3230,10 +3230,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3249,10 +3249,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3268,10 +3268,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3287,8 +3287,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3301,10 +3301,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3351,60 +3351,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3416,11 +3416,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3495,60 +3495,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3557,10 +3557,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3575,10 +3575,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3594,10 +3594,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3613,10 +3613,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3632,10 +3632,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3651,10 +3651,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3670,8 +3670,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3734,60 +3734,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3799,11 +3799,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3831,6 +3831,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3847,30 +3871,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3902,63 +3902,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3968,10 +3968,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3986,10 +3986,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4005,10 +4005,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4024,10 +4024,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4043,8 +4043,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4060,8 +4060,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4077,8 +4077,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4091,10 +4091,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4141,72 +4141,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4281,60 +4281,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4343,10 +4343,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4361,10 +4361,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4380,10 +4380,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4399,10 +4399,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4418,8 +4418,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4435,8 +4435,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4452,8 +4452,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4466,10 +4466,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4516,58 +4516,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4577,11 +4577,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4609,16 +4609,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4631,24 +4639,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
12.06.19 Today Last Sales Updated 10:51 PM
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 11.06.19</t>
+    <t>Date: 12.06.19</t>
   </si>
 </sst>
 </file>
@@ -283,38 +283,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -325,6 +298,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -332,9 +335,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,14 +2253,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2273,24 +2283,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>43</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>73</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>43000</v>
+        <v>73000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>212</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>236</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>106000</v>
+        <v>118000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>214</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>69</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>21400</v>
+        <v>6900</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,13 +2462,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
-        <v>132</v>
-      </c>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23">
+        <v>2</v>
+      </c>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>6600</v>
+        <v>100</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2481,8 +2481,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2498,8 +2498,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2512,14 +2512,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>177000</v>
+        <v>198000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2562,58 +2562,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2623,9 +2623,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2712,60 +2712,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2774,10 +2774,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2792,13 +2792,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="21">
-        <v>43</v>
-      </c>
-      <c r="F33" s="21"/>
+      <c r="E33" s="23">
+        <v>73</v>
+      </c>
+      <c r="F33" s="23"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>43000</v>
+        <v>73000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2811,13 +2811,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="21">
-        <v>212</v>
-      </c>
-      <c r="F34" s="21"/>
+      <c r="E34" s="23">
+        <v>236</v>
+      </c>
+      <c r="F34" s="23"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>106000</v>
+        <v>118000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2830,13 +2830,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="21">
-        <v>214</v>
-      </c>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23">
+        <v>69</v>
+      </c>
+      <c r="F35" s="23"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>21400</v>
+        <v>6900</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2849,13 +2849,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="21">
-        <v>132</v>
-      </c>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23">
+        <v>2</v>
+      </c>
+      <c r="F36" s="23"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>6600</v>
+        <v>100</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2868,8 +2868,8 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -2885,8 +2885,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2899,14 +2899,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>177000</v>
+        <v>198000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2949,58 +2949,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3010,9 +3010,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3040,28 +3040,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3078,6 +3056,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3108,63 +3108,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3174,10 +3174,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3192,10 +3192,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3211,10 +3211,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3230,10 +3230,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3249,10 +3249,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3268,10 +3268,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3287,8 +3287,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3301,10 +3301,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3351,60 +3351,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3416,11 +3416,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3495,60 +3495,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3557,10 +3557,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3575,10 +3575,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3594,10 +3594,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3613,10 +3613,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3632,10 +3632,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3651,10 +3651,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3670,8 +3670,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3734,60 +3734,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3799,11 +3799,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3831,30 +3831,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3871,6 +3847,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3902,63 +3902,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3968,10 +3968,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3986,10 +3986,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4005,10 +4005,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4024,10 +4024,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4043,8 +4043,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4060,8 +4060,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4077,8 +4077,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4091,10 +4091,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4141,72 +4141,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4281,60 +4281,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4343,10 +4343,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4361,10 +4361,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4380,10 +4380,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4399,10 +4399,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4418,8 +4418,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4435,8 +4435,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4452,8 +4452,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4466,10 +4466,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4516,58 +4516,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4577,11 +4577,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4609,6 +4609,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4621,34 +4649,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
13.06.19 Today sales 8:02 PM
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 12.06.19</t>
+    <t>Date: 13.06.19</t>
   </si>
 </sst>
 </file>
@@ -283,11 +283,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -298,36 +325,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,6 +332,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,6 +2253,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2265,32 +2291,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H47" sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>73</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>56</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>73000</v>
+        <v>56000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>236</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>68</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>118000</v>
+        <v>34000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>69</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>169</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>6900</v>
+        <v>16900</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,10 +2462,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -2481,11 +2481,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21">
+        <v>50</v>
+      </c>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2498,8 +2500,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2512,14 +2514,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>198000</v>
+        <v>108000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2562,58 +2564,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2623,9 +2625,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2712,60 +2714,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2774,10 +2776,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2792,13 +2794,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="23">
-        <v>73</v>
-      </c>
-      <c r="F33" s="23"/>
+      <c r="E33" s="21">
+        <v>56</v>
+      </c>
+      <c r="F33" s="21"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>73000</v>
+        <v>56000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2811,13 +2813,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="23">
-        <v>236</v>
-      </c>
-      <c r="F34" s="23"/>
+      <c r="E34" s="21">
+        <v>68</v>
+      </c>
+      <c r="F34" s="21"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>118000</v>
+        <v>34000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2830,13 +2832,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="23">
-        <v>69</v>
-      </c>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21">
+        <v>169</v>
+      </c>
+      <c r="F35" s="21"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>6900</v>
+        <v>16900</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2849,10 +2851,10 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="21">
         <v>2</v>
       </c>
-      <c r="F36" s="23"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2868,11 +2870,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34">
+        <v>50</v>
+      </c>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2885,8 +2889,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2899,14 +2903,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>198000</v>
+        <v>108000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2949,58 +2953,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3010,9 +3014,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3040,6 +3044,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3056,28 +3082,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3108,63 +3112,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3174,10 +3178,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3192,10 +3196,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3211,10 +3215,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3230,10 +3234,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3249,10 +3253,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3268,10 +3272,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3287,8 +3291,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3301,10 +3305,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3351,60 +3355,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3416,11 +3420,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3495,60 +3499,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3557,10 +3561,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3575,10 +3579,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3594,10 +3598,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3613,10 +3617,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3632,10 +3636,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3651,10 +3655,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3670,8 +3674,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3734,60 +3738,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3799,11 +3803,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3831,6 +3835,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3847,30 +3875,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3902,63 +3906,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3968,10 +3972,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3986,10 +3990,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4005,10 +4009,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4024,10 +4028,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4043,8 +4047,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4060,8 +4064,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4077,8 +4081,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4091,10 +4095,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4141,72 +4145,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4281,60 +4285,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4343,10 +4347,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4361,10 +4365,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4380,10 +4384,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4399,10 +4403,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4418,8 +4422,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4435,8 +4439,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4452,8 +4456,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4466,10 +4470,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4516,58 +4520,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4577,11 +4581,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4609,16 +4613,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4631,24 +4643,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
15.06.19 Today Sales Updated 9:35 PM
</commit_message>
<xml_diff>
--- a/May/Othes/Cash.xlsx
+++ b/May/Othes/Cash.xlsx
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 13.06.19</t>
+    <t>Date: 15.06.19</t>
   </si>
 </sst>
 </file>
@@ -283,38 +283,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -325,6 +298,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -332,9 +335,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1546,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1608,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1626,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1645,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1664,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1683,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1702,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1719,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1733,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1783,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1844,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1923,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1985,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2022,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2041,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2060,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2079,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2096,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2110,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2160,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2221,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,14 +2253,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2273,24 +2283,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2321,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>56</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>54</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>56000</v>
+        <v>54000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>68</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>202</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>34000</v>
+        <v>101000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>169</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>270</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>16900</v>
+        <v>27000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,13 +2462,11 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
-        <v>2</v>
-      </c>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2481,13 +2479,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
-        <v>50</v>
-      </c>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2500,8 +2496,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2514,14 +2510,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>108000</v>
+        <v>182000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2564,58 +2560,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2625,9 +2621,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2714,60 +2710,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2776,10 +2772,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2794,13 +2790,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="21">
-        <v>56</v>
-      </c>
-      <c r="F33" s="21"/>
+      <c r="E33" s="23">
+        <v>54</v>
+      </c>
+      <c r="F33" s="23"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>56000</v>
+        <v>54000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2813,13 +2809,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="21">
-        <v>68</v>
-      </c>
-      <c r="F34" s="21"/>
+      <c r="E34" s="23">
+        <v>202</v>
+      </c>
+      <c r="F34" s="23"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>34000</v>
+        <v>101000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2832,13 +2828,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="21">
-        <v>169</v>
-      </c>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23">
+        <v>270</v>
+      </c>
+      <c r="F35" s="23"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>16900</v>
+        <v>27000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2851,13 +2847,11 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="21">
-        <v>2</v>
-      </c>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2870,13 +2864,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34">
-        <v>50</v>
-      </c>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2889,8 +2881,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2903,14 +2895,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>108000</v>
+        <v>182000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2953,58 +2945,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3014,9 +3006,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3044,28 +3036,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3082,6 +3052,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3112,63 +3104,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3178,10 +3170,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3196,10 +3188,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3215,10 +3207,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3234,10 +3226,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3253,10 +3245,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3272,10 +3264,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3291,8 +3283,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3305,10 +3297,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3355,60 +3347,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3420,11 +3412,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3499,60 +3491,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3561,10 +3553,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3579,10 +3571,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3598,10 +3590,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3617,10 +3609,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3636,10 +3628,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3655,10 +3647,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3674,8 +3666,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3738,60 +3730,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3803,11 +3795,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3835,30 +3827,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3875,6 +3843,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3906,63 +3898,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3972,10 +3964,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3990,10 +3982,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4009,10 +4001,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4028,10 +4020,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4047,8 +4039,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4064,8 +4056,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4081,8 +4073,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4095,10 +4087,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4145,72 +4137,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4285,60 +4277,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4347,10 +4339,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4365,10 +4357,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4384,10 +4376,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4403,10 +4395,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4422,8 +4414,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4439,8 +4431,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4456,8 +4448,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4470,10 +4462,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4520,58 +4512,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4581,11 +4573,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4613,6 +4605,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4625,34 +4645,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>